<commit_message>
mean anomaly neptune moons
</commit_message>
<xml_diff>
--- a/src/app/scene/data/neptune.xlsx
+++ b/src/app/scene/data/neptune.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl03940s\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl03940s\Documents\GitHub\solar-system\src\app\scene\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Order</t>
   </si>
@@ -156,13 +156,55 @@
   </si>
   <si>
     <t>Neso</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>334.9</t>
+  </si>
+  <si>
+    <t>193.6</t>
+  </si>
+  <si>
+    <t>319.6</t>
+  </si>
+  <si>
+    <t>187.1</t>
+  </si>
+  <si>
+    <t>34.9</t>
+  </si>
+  <si>
+    <t>114.2</t>
+  </si>
+  <si>
+    <t>264.8</t>
+  </si>
+  <si>
+    <t>359.3</t>
+  </si>
+  <si>
+    <t>96.8</t>
+  </si>
+  <si>
+    <t>129.4</t>
+  </si>
+  <si>
+    <t>321.1</t>
+  </si>
+  <si>
+    <t>206.2</t>
+  </si>
+  <si>
+    <t>269.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +239,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF888888"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00FF00"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -296,7 +368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -388,6 +460,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -397,7 +470,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -682,7 +772,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H17"/>
+      <selection activeCell="L4" sqref="L4:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +781,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -711,7 +801,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -727,13 +817,16 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="3"/>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
       <c r="H3" t="s">
         <v>32</v>
       </c>
@@ -769,6 +862,9 @@
       <c r="F4" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="G4" s="35" t="s">
+        <v>45</v>
+      </c>
       <c r="H4" t="str">
         <f>UPPER(SUBSTITUTE(SUBSTITUTE(B4," ","_"),"/","_"))</f>
         <v>NAIAD</v>
@@ -777,7 +873,7 @@
         <f>LOWER(SUBSTITUTE(SUBSTITUTE(B4," ","-"),"/","/"))</f>
         <v>naiad</v>
       </c>
-      <c r="J4" s="34" t="str">
+      <c r="J4" s="31" t="str">
         <f>SUBSTITUTE(C4/2,",",".")</f>
         <v>30.2</v>
       </c>
@@ -798,7 +894,7 @@
   semiMajorAxis: "&amp;E4&amp;",
   eccentricity: "&amp;F4&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G4&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -816,7 +912,7 @@
   semiMajorAxis: 48224,
   eccentricity: 0.0047,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 334.9,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -843,6 +939,9 @@
       <c r="F5" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="G5" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="H5" t="str">
         <f t="shared" ref="H5:H17" si="0">UPPER(SUBSTITUTE(SUBSTITUTE(B5," ","_"),"/","_"))</f>
         <v>THALASSA</v>
@@ -851,7 +950,7 @@
         <f t="shared" ref="I5:I17" si="1">LOWER(SUBSTITUTE(SUBSTITUTE(B5," ","-"),"/","/"))</f>
         <v>thalassa</v>
       </c>
-      <c r="J5" s="34" t="str">
+      <c r="J5" s="31" t="str">
         <f t="shared" ref="J5:J17" si="2">SUBSTITUTE(C5/2,",",".")</f>
         <v>40.7</v>
       </c>
@@ -872,7 +971,7 @@
   semiMajorAxis: "&amp;E5&amp;",
   eccentricity: "&amp;F5&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G5&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -890,7 +989,7 @@
   semiMajorAxis: 50074,
   eccentricity: 0.0018,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 193.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -917,6 +1016,9 @@
       <c r="F6" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="G6" s="35" t="s">
+        <v>47</v>
+      </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>DESPINA</v>
@@ -925,7 +1027,7 @@
         <f t="shared" si="1"/>
         <v>despina</v>
       </c>
-      <c r="J6" s="34" t="str">
+      <c r="J6" s="31" t="str">
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
@@ -947,7 +1049,7 @@
   semiMajorAxis: 52526,
   eccentricity: 0.0004,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 319.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -974,6 +1076,9 @@
       <c r="F7" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="G7" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>GALATEA</v>
@@ -982,7 +1087,7 @@
         <f t="shared" si="1"/>
         <v>galatea</v>
       </c>
-      <c r="J7" s="34" t="str">
+      <c r="J7" s="31" t="str">
         <f t="shared" si="2"/>
         <v>87.4</v>
       </c>
@@ -1004,7 +1109,7 @@
   semiMajorAxis: 61953,
   eccentricity: 0.0001,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 187.1,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1031,6 +1136,9 @@
       <c r="F8" s="9" t="s">
         <v>21</v>
       </c>
+      <c r="G8" s="35" t="s">
+        <v>49</v>
+      </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>LARISSA</v>
@@ -1039,7 +1147,7 @@
         <f t="shared" si="1"/>
         <v>larissa</v>
       </c>
-      <c r="J8" s="34" t="str">
+      <c r="J8" s="31" t="str">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
@@ -1061,7 +1169,7 @@
   semiMajorAxis: 73548,
   eccentricity: 0.0012,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 34.9,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1088,6 +1196,9 @@
       <c r="F9" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="G9" s="36">
+        <v>0</v>
+      </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>HIPPOCAMP</v>
@@ -1096,7 +1207,7 @@
         <f t="shared" si="1"/>
         <v>hippocamp</v>
       </c>
-      <c r="J9" s="34" t="str">
+      <c r="J9" s="31" t="str">
         <f t="shared" si="2"/>
         <v>17.4</v>
       </c>
@@ -1118,7 +1229,7 @@
   semiMajorAxis: 105283,
   eccentricity: 0.0005,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 0,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1145,6 +1256,9 @@
       <c r="F10" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="G10" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>PROTEUS</v>
@@ -1153,7 +1267,7 @@
         <f t="shared" si="1"/>
         <v>proteus</v>
       </c>
-      <c r="J10" s="34" t="str">
+      <c r="J10" s="31" t="str">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
@@ -1175,7 +1289,7 @@
   semiMajorAxis: 117646,
   eccentricity: 0.0005,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 114.2,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1202,6 +1316,9 @@
       <c r="F11" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="G11" s="37" t="s">
+        <v>51</v>
+      </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>TRITON</v>
@@ -1210,7 +1327,7 @@
         <f t="shared" si="1"/>
         <v>triton</v>
       </c>
-      <c r="J11" s="34" t="str">
+      <c r="J11" s="31" t="str">
         <f t="shared" si="2"/>
         <v>1352.6</v>
       </c>
@@ -1232,7 +1349,7 @@
   semiMajorAxis: 354759,
   eccentricity: 0.0000,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 264.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1259,6 +1376,9 @@
       <c r="F12" s="21" t="s">
         <v>26</v>
       </c>
+      <c r="G12" s="38" t="s">
+        <v>52</v>
+      </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>NEREID</v>
@@ -1267,7 +1387,7 @@
         <f t="shared" si="1"/>
         <v>nereid</v>
       </c>
-      <c r="J12" s="34" t="str">
+      <c r="J12" s="31" t="str">
         <f t="shared" si="2"/>
         <v>178.5</v>
       </c>
@@ -1289,7 +1409,7 @@
   semiMajorAxis: 5513800,
   eccentricity: 0.7507,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 359.3,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1316,6 +1436,9 @@
       <c r="F13" s="17" t="s">
         <v>27</v>
       </c>
+      <c r="G13" s="39" t="s">
+        <v>53</v>
+      </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>HALIMEDE</v>
@@ -1324,7 +1447,7 @@
         <f t="shared" si="1"/>
         <v>halimede</v>
       </c>
-      <c r="J13" s="34" t="str">
+      <c r="J13" s="31" t="str">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
@@ -1346,7 +1469,7 @@
   semiMajorAxis: 16681000,
   eccentricity: 0.2909,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 96.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1373,6 +1496,9 @@
       <c r="F14" s="25" t="s">
         <v>28</v>
       </c>
+      <c r="G14" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>SAO</v>
@@ -1381,7 +1507,7 @@
         <f t="shared" si="1"/>
         <v>sao</v>
       </c>
-      <c r="J14" s="34" t="str">
+      <c r="J14" s="31" t="str">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
@@ -1403,7 +1529,7 @@
   semiMajorAxis: 22619000,
   eccentricity: 0.2827,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 129.4,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1430,6 +1556,9 @@
       <c r="F15" s="25" t="s">
         <v>29</v>
       </c>
+      <c r="G15" s="40" t="s">
+        <v>55</v>
+      </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>LAOMEDEIA</v>
@@ -1438,7 +1567,7 @@
         <f t="shared" si="1"/>
         <v>laomedeia</v>
       </c>
-      <c r="J15" s="34" t="str">
+      <c r="J15" s="31" t="str">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
@@ -1460,7 +1589,7 @@
   semiMajorAxis: 23613000,
   eccentricity: 0.4339,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 321.1,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1487,6 +1616,9 @@
       <c r="F16" s="29" t="s">
         <v>30</v>
       </c>
+      <c r="G16" s="39" t="s">
+        <v>56</v>
+      </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>PSAMATHE</v>
@@ -1495,7 +1627,7 @@
         <f t="shared" si="1"/>
         <v>psamathe</v>
       </c>
-      <c r="J16" s="34" t="str">
+      <c r="J16" s="31" t="str">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -1517,7 +1649,7 @@
   semiMajorAxis: 46705000,
   eccentricity: 0.4617,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 206.2,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1544,6 +1676,9 @@
       <c r="F17" s="29" t="s">
         <v>31</v>
       </c>
+      <c r="G17" s="39" t="s">
+        <v>57</v>
+      </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
         <v>NESO</v>
@@ -1552,7 +1687,7 @@
         <f t="shared" si="1"/>
         <v>neso</v>
       </c>
-      <c r="J17" s="34" t="str">
+      <c r="J17" s="31" t="str">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
@@ -1574,7 +1709,7 @@
   semiMajorAxis: 50258000,
   eccentricity: 0.4243,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 269.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null

</xml_diff>